<commit_message>
Added some Data Analysis
</commit_message>
<xml_diff>
--- a/Ising_Results.xlsx
+++ b/Ising_Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mharkess-adm\Downloads\Paralyzed-Icing-Modle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD824D6E-A538-4417-9814-E6602FC1F4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771D0DC8-08D1-4008-8059-4F055E318F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6900" yWindow="2445" windowWidth="21900" windowHeight="12435" xr2:uid="{7AB5D500-91B4-4F98-AF75-B433A2971F8E}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="16">
   <si>
     <t>File</t>
   </si>
@@ -72,6 +72,21 @@
   </si>
   <si>
     <t>Ising_Wolff_Parallel</t>
+  </si>
+  <si>
+    <t>Speedup (1:4)</t>
+  </si>
+  <si>
+    <t>Speedup (1:8)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Efficency (Speed: 4 Thread)</t>
+  </si>
+  <si>
+    <t>Efficency (Speed: 8 Thread)</t>
   </si>
 </sst>
 </file>
@@ -423,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D923F44-56B7-4AFF-B150-F34F74D3B03E}">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,9 +452,13 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="29.5703125" customWidth="1"/>
+    <col min="10" max="10" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -458,8 +477,20 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -478,8 +509,14 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -498,8 +535,24 @@
       <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="0">E3/E7</f>
+        <v>1.0060606060606061</v>
+      </c>
+      <c r="H3">
+        <f>E3/E10</f>
+        <v>1.0060606060606061</v>
+      </c>
+      <c r="I3">
+        <f>G3/4</f>
+        <v>0.25151515151515152</v>
+      </c>
+      <c r="J3">
+        <f>H3/8</f>
+        <v>0.12575757575757576</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -518,8 +571,24 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.98200899550224885</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H5" si="1">E4/E11</f>
+        <v>0.98496240601503759</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I5" si="2">G4/4</f>
+        <v>0.24550224887556221</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J5" si="3">H4/8</f>
+        <v>0.1231203007518797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -538,8 +607,24 @@
       <c r="F5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>0.98009950248756217</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0.97561904761904761</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>0.24502487562189054</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="3"/>
+        <v>0.12195238095238095</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -559,7 +644,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -579,7 +664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -599,7 +684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -619,7 +704,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -639,7 +724,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -659,7 +744,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -679,7 +764,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -698,8 +783,14 @@
       <c r="F13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -718,8 +809,24 @@
       <c r="F14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f>E14/E18</f>
+        <v>1.0535714285714286</v>
+      </c>
+      <c r="H14">
+        <f>E14/E21</f>
+        <v>1.0727272727272728</v>
+      </c>
+      <c r="I14">
+        <f>G14/4</f>
+        <v>0.26339285714285715</v>
+      </c>
+      <c r="J14">
+        <f>H14/8</f>
+        <v>0.13409090909090909</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -738,8 +845,24 @@
       <c r="F15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f t="shared" ref="G15:G16" si="4">E15/E19</f>
+        <v>0.95625942684766219</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ref="H15:H16" si="5">E15/E22</f>
+        <v>0.95481927710843373</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ref="I15:I16" si="6">G15/4</f>
+        <v>0.23906485671191555</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ref="J15:J16" si="7">H15/8</f>
+        <v>0.11935240963855422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -758,8 +881,24 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>0.9752192146397255</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="5"/>
+        <v>0.96893939393939399</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>0.24380480365993137</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="7"/>
+        <v>0.12111742424242425</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -779,7 +918,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -799,7 +938,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -819,7 +958,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -839,7 +978,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -859,7 +998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -879,7 +1018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -899,7 +1038,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -918,8 +1057,14 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -938,8 +1083,24 @@
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <f>E25/E29</f>
+        <v>0.38519764507989906</v>
+      </c>
+      <c r="H25">
+        <f>E25/E32</f>
+        <v>0.28482587064676618</v>
+      </c>
+      <c r="I25">
+        <f>G25/4</f>
+        <v>9.6299411269974766E-2</v>
+      </c>
+      <c r="J25">
+        <f>H25/8</f>
+        <v>3.5603233830845772E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>4</v>
       </c>
@@ -958,8 +1119,24 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <f t="shared" ref="G26:G27" si="8">E26/E30</f>
+        <v>0.39630434782608698</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ref="H26:H27" si="9">E26/E33</f>
+        <v>0.3000329163923634</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:I27" si="10">G26/4</f>
+        <v>9.9076086956521744E-2</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26:J27" si="11">H26/8</f>
+        <v>3.7504114549045425E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -978,8 +1155,24 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="8"/>
+        <v>0.42780019321475249</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="9"/>
+        <v>0.31413787347688199</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="10"/>
+        <v>0.10695004830368812</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="11"/>
+        <v>3.9267234184610249E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -999,7 +1192,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1019,7 +1212,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -1039,7 +1232,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1252,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1099,7 +1292,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1119,7 +1312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
@@ -1138,8 +1331,14 @@
       <c r="F35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1158,8 +1357,24 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f>E36/E40</f>
+        <v>0.35492700729927007</v>
+      </c>
+      <c r="H36">
+        <f>E36/E43</f>
+        <v>0.27706552706552706</v>
+      </c>
+      <c r="I36">
+        <f>G36/4</f>
+        <v>8.8731751824817517E-2</v>
+      </c>
+      <c r="J36">
+        <f>H36/8</f>
+        <v>3.4633190883190883E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1178,8 +1393,24 @@
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f t="shared" ref="G37:G38" si="12">E37/E41</f>
+        <v>0.36050895381715364</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ref="H37:H38" si="13">E37/E44</f>
+        <v>0.27151730257320317</v>
+      </c>
+      <c r="I37">
+        <f t="shared" ref="I37:I38" si="14">G37/4</f>
+        <v>9.0127238454288411E-2</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ref="J37:J38" si="15">H37/8</f>
+        <v>3.3939662821650396E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1198,8 +1429,24 @@
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f t="shared" si="12"/>
+        <v>0.36376520609424828</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="13"/>
+        <v>0.27742749054224464</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="14"/>
+        <v>9.0941301523562071E-2</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="15"/>
+        <v>3.467843631778058E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1219,7 +1466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -1239,7 +1486,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1259,7 +1506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1279,7 +1526,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -1299,7 +1546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1566,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -1339,7 +1586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1358,8 +1605,14 @@
       <c r="F46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>10</v>
       </c>
@@ -1378,8 +1631,24 @@
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f>E47/E51</f>
+        <v>0.99628252788104088</v>
+      </c>
+      <c r="H47">
+        <f>E47/E54</f>
+        <v>1.0229007633587786</v>
+      </c>
+      <c r="I47">
+        <f>G47/4</f>
+        <v>0.24907063197026022</v>
+      </c>
+      <c r="J47">
+        <f>H47/8</f>
+        <v>0.12786259541984732</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -1398,8 +1667,24 @@
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f t="shared" ref="G48:G49" si="16">E48/E52</f>
+        <v>1.0185004868549172</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ref="H48:H49" si="17">E48/E55</f>
+        <v>1.0125847047434657</v>
+      </c>
+      <c r="I48">
+        <f t="shared" ref="I48:I49" si="18">G48/4</f>
+        <v>0.25462512171372931</v>
+      </c>
+      <c r="J48">
+        <f t="shared" ref="J48:J50" si="19">H48/8</f>
+        <v>0.12657308809293322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>10</v>
       </c>
@@ -1418,8 +1703,24 @@
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f t="shared" si="16"/>
+        <v>0.99586173320350535</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="17"/>
+        <v>0.99756157034869541</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="18"/>
+        <v>0.24896543330087634</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="19"/>
+        <v>0.12469519629358693</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>10</v>
       </c>
@@ -1439,7 +1740,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>10</v>
       </c>
@@ -1459,7 +1760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -1479,7 +1780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -1499,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>10</v>
       </c>
@@ -1519,7 +1820,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>10</v>
       </c>
@@ -1539,7 +1840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>

</xml_diff>